<commit_message>
Some updated, some added v2
</commit_message>
<xml_diff>
--- a/6.1.Desyukevich.xlsx
+++ b/6.1.Desyukevich.xlsx
@@ -11,9 +11,10 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="6_1_1" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="6_1_2" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="6_1_3" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="6_1_5" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="6_1_6" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="6_1_7" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="6_1_4" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="6_1_5" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="6_1_6" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="6_1_7" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -645,6 +646,48 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>intersection</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -671,11 +714,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Мафия</t>
+          <t>Party</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>8.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
@@ -684,11 +727,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Карточная</t>
+          <t>Мафия</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>4.5</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="4">
@@ -697,11 +740,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Семейная</t>
+          <t>Карточная</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="5">
@@ -710,11 +753,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Party</t>
+          <t>Семейная</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -735,7 +778,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3135,7 +3178,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>